<commit_message>
changes for person mandate data
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdatafiles/STGAMO.xlsx
+++ b/src/main/resources/Testdatafiles/STGAMO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="DCF01" sheetId="1" state="visible" r:id="rId2"/>
@@ -296,13 +296,13 @@
     <t xml:space="preserve">Create/Prepare Pre Charge Decision</t>
   </si>
   <si>
-    <t xml:space="preserve">Forename 1</t>
+    <t xml:space="preserve">Forename1</t>
   </si>
   <si>
     <t xml:space="preserve">Surname</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of Birth</t>
+    <t xml:space="preserve">Birth</t>
   </si>
   <si>
     <t xml:space="preserve">Defandant</t>
@@ -465,7 +465,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="46.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -593,7 +593,7 @@
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -639,7 +639,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -683,7 +683,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.1"/>
   </cols>
@@ -778,14 +778,14 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.47"/>
   </cols>
   <sheetData>
@@ -847,11 +847,11 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
   </cols>
@@ -900,7 +900,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="46.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -946,7 +946,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.35"/>
@@ -1059,7 +1059,7 @@
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="24.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1234,7 +1234,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1328,7 +1328,7 @@
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1403,7 +1403,7 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1451,7 +1451,7 @@
       <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="42.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="42.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1503,7 +1503,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>